<commit_message>
a bunch of bom stuff
</commit_message>
<xml_diff>
--- a/cansatBrain planning.xlsx
+++ b/cansatBrain planning.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="power estimation" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="120">
   <si>
     <t xml:space="preserve">device</t>
   </si>
@@ -363,6 +363,12 @@
     <t xml:space="preserve">placed</t>
   </si>
   <si>
+    <t xml:space="preserve">no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">snapeda</t>
+  </si>
+  <si>
     <t xml:space="preserve">yes</t>
   </si>
   <si>
@@ -370,6 +376,9 @@
   </si>
   <si>
     <t xml:space="preserve">online</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DM3CS-SF</t>
   </si>
   <si>
     <t xml:space="preserve">3 pin header</t>
@@ -561,12 +570,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="5" min="2" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="5" min="2" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -840,16 +849,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="5" min="2" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="30.3724489795918"/>
-    <col collapsed="false" hidden="false" max="14" min="11" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="32.3979591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="5" min="2" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="30.1020408163265"/>
+    <col collapsed="false" hidden="false" max="14" min="11" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="31.9948979591837"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1129,11 +1138,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="45.4897959183674"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="46.1683673469388"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="78.4285714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="44.8163265306122"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="45.6275510204082"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="77.484693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.2602040816327"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1295,9 +1304,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="10.6632653061225"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1449,7 +1458,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.0714285714286"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1501,16 +1510,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.0714285714286"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1537,7 +1546,7 @@
         <v>13</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>10</v>
@@ -1548,7 +1557,7 @@
         <v>17</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>10</v>
@@ -1559,7 +1568,7 @@
         <v>19</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>10</v>
@@ -1570,10 +1579,13 @@
         <v>21</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>10</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1592,7 +1604,7 @@
         <v>28</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>10</v>
@@ -1603,7 +1615,7 @@
         <v>29</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>10</v>

</xml_diff>